<commit_message>
start met het 2de testrapport
</commit_message>
<xml_diff>
--- a/meetrapporten/working/resultaten stepToIntensityImage/vergelijking.xlsx
+++ b/meetrapporten/working/resultaten stepToIntensityImage/vergelijking.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ti-software\HU-Vision-1819-Bas-Lennart\meetrapporten\working\resultaten stepToIntensityImage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCED7FA5-7E34-4F1D-A927-F0125DED3141}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838C3B18-0ECB-47EB-B2DD-232E68238D8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FBFE720-8F39-4D5B-AE7A-9E3706495CDB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="2" xr2:uid="{0FBFE720-8F39-4D5B-AE7A-9E3706495CDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="default" sheetId="3" r:id="rId1"/>
+    <sheet name="nauwkeurigheid" sheetId="3" r:id="rId1"/>
     <sheet name="samenvatting" sheetId="6" r:id="rId2"/>
+    <sheet name="snelheid" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneGegevens_1" localSheetId="0" hidden="1">default!$A$1:$B$17</definedName>
+    <definedName name="ExterneGegevens_1" localSheetId="0" hidden="1">nauwkeurigheid!$A$1:$B$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>1</t>
   </si>
@@ -136,6 +137,21 @@
   </si>
   <si>
     <t>Luminosity</t>
+  </si>
+  <si>
+    <t>Test-ID</t>
+  </si>
+  <si>
+    <t>Computer1:</t>
+  </si>
+  <si>
+    <t>Computer2:</t>
+  </si>
+  <si>
+    <t>Computer3:</t>
+  </si>
+  <si>
+    <t>test3/test1</t>
   </si>
 </sst>
 </file>
@@ -237,6 +253,23 @@
     <tableColumn id="2" xr3:uid="{03D0F49D-DF5E-4481-A77A-8E591310BD19}" name="totaal verschil facial parameters" totalsRowFunction="count"/>
     <tableColumn id="3" xr3:uid="{A92019BC-2216-43E5-9114-2B70B78B4D92}" name="grootste verschil facial parameters"/>
     <tableColumn id="5" xr3:uid="{119B900C-064C-4B05-B81B-BE3C03BDC0D3}" name="aantal verschillen "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C0772DD-3EB7-4443-AFF6-C00894C20E54}" name="Tabel12" displayName="Tabel12" ref="A1:D5" totalsRowCount="1">
+  <autoFilter ref="A1:D4" xr:uid="{F9C8795C-5284-40C2-A43C-81B9DA4BBEEB}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{979B31E0-C43B-4DAC-845E-F014B172D370}" name="Test-ID" totalsRowLabel="test3/test1"/>
+    <tableColumn id="2" xr3:uid="{DB8CDF68-241A-4F22-B407-AF17974BF6AD}" name="Computer1:" totalsRowFunction="custom">
+      <totalsRowFormula>B4/B2</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{38F7E89E-4397-4D0B-95AE-3C0BA5779106}" name="Computer2:" totalsRowFunction="custom">
+      <totalsRowFormula>C4/C2</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{7A06954F-E173-47FD-852E-4281A0DF1DE3}" name="Computer3:"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -541,19 +574,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AF8D9-0AD9-4527-AE10-C805E06DB5A7}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -570,7 +603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -587,7 +620,7 @@
         <v>1.54541</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -604,7 +637,7 @@
         <v>0.57958600000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -621,7 +654,7 @@
         <v>0.71213899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -638,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -655,7 +688,7 @@
         <v>2.1597300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -672,7 +705,7 @@
         <v>1.22299</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -689,7 +722,7 @@
         <v>0.38050600000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -706,7 +739,7 @@
         <v>1.7418100000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -723,7 +756,7 @@
         <v>0.44695299999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -740,7 +773,7 @@
         <v>9.4509200000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -757,7 +790,7 @@
         <v>0.25561</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -774,7 +807,7 @@
         <v>0.270646</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -791,7 +824,7 @@
         <v>0.22553799999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -808,7 +841,7 @@
         <v>0.75179499999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -825,7 +858,7 @@
         <v>1.55986</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -855,18 +888,18 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -880,7 +913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -894,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -908,7 +941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -926,6 +959,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AFB634-1258-4BE4-8776-77B5C63DE7D3}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2057</v>
+      </c>
+      <c r="C2">
+        <v>5694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2538</v>
+      </c>
+      <c r="C3">
+        <v>13090</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10911</v>
+      </c>
+      <c r="C4">
+        <v>29199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f>B4/B2</f>
+        <v>5.3043266893534273</v>
+      </c>
+      <c r="C5">
+        <f>C4/C2</f>
+        <v>5.1280295047418338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>